<commit_message>
Only changed if number of rows has been added
</commit_message>
<xml_diff>
--- a/uploads/uploadexcel-items.xlsx
+++ b/uploads/uploadexcel-items.xlsx
@@ -306,7 +306,57 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1016"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2" table:number-rows-repeated="1048566">
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A01AA01009</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Sodium Chloride</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>WHITEDENT TOOTHPASTE 23ml/TBE</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>DT</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>BOX</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2060" calcext:value-type="float">
+            <text:p>2060</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NEW</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1016"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A01AA01010</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Sodium Chloride</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>BUBLBE GUM </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>DT</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>BOX</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2060" calcext:value-type="float">
+            <text:p>2060</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NEW</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1016"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2" table:number-rows-repeated="1048564">
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
@@ -323,11 +373,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2022-07-25T08:21:57.585355338</meta:creation-date>
-    <dc:date>2022-07-25T14:18:54.925487819</dc:date>
-    <meta:editing-duration>PT2H33M18S</meta:editing-duration>
-    <meta:editing-cycles>6</meta:editing-cycles>
+    <dc:date>2022-07-25T17:45:29.061665731</dc:date>
+    <meta:editing-duration>PT3H30M41S</meta:editing-duration>
+    <meta:editing-cycles>8</meta:editing-cycles>
     <meta:generator>LibreOffice/7.3.5.2$Linux_X86_64 LibreOffice_project/392c644e8a6d1ea0765aa2d613a91bcef808d6ea</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="66" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="80" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -339,13 +389,13 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">42233</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">5170</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">6309</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">2</config:config-item>
               <config:config-item config:name="CursorPositionY" config:type="int">10</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
@@ -407,7 +457,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">pAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAxQAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6TGV0dGVyAAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2Zm</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">pAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAxQAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6TGV0dGVyAER1cGxleDpOb25lAAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2Zm</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>

</xml_diff>